<commit_message>
commiting latest code with homepage test cases
</commit_message>
<xml_diff>
--- a/MenuList.xlsx
+++ b/MenuList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>THE EDIT</t>
   </si>
@@ -41,15 +41,6 @@
     <t>ACCESSORIES</t>
   </si>
   <si>
-    <t>LOOKBOOKS</t>
-  </si>
-  <si>
-    <t>SALE</t>
-  </si>
-  <si>
-    <t>SS'20 EDIT</t>
-  </si>
-  <si>
     <t>MenuList</t>
   </si>
   <si>
@@ -210,6 +201,21 @@
   </si>
   <si>
     <t>NEW IN</t>
+  </si>
+  <si>
+    <t>LOUNGEWEAR</t>
+  </si>
+  <si>
+    <t>MASKS</t>
+  </si>
+  <si>
+    <t>FAB FREEDOM SALE</t>
+  </si>
+  <si>
+    <t>GIFT CARD</t>
+  </si>
+  <si>
+    <t>FAB FIX</t>
   </si>
 </sst>
 </file>
@@ -554,7 +560,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -562,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -575,12 +581,12 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -615,17 +621,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +664,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -658,72 +674,72 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -746,187 +762,187 @@
   <sheetData>
     <row r="1" spans="1:1" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>